<commit_message>
Added more cases to GetCellValues
Added more cases and a new field to model with decimal data type to load accounting data

Updated the xlsx to add Debt header and values with accounting as data type
</commit_message>
<xml_diff>
--- a/test/Excel.IO.Test/Resources/test2.xlsx
+++ b/test/Excel.IO.Test/Resources/test2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiscox-my.sharepoint.com/personal/joao_dinis_hiscox_com/Documents/Documents/GitHub/Excel-IO/test/Excel.IO.Test/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinisj\OneDrive - Hiscox\Documents\GitHub\Excel-IO\test\Excel.IO.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA2568E7-84B2-4FAE-8309-597935BCE867}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{BA2568E7-84B2-4FAE-8309-597935BCE867}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{86797C8C-F96D-4435-9513-F58AD3556A5D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="14370" xr2:uid="{68AEA8F3-490C-4032-82EA-9294EAAABB5A}"/>
+    <workbookView xWindow="1860" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{68AEA8F3-490C-4032-82EA-9294EAAABB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>Age</t>
   </si>
@@ -233,13 +233,17 @@
   </si>
   <si>
     <t>Something</t>
+  </si>
+  <si>
+    <t>Debt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="[&lt;=999999999]###\ ###\ ###;\(###\)\ ###\ ###\ ###"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
@@ -293,7 +297,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -307,6 +311,7 @@
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -623,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3072FA3-C783-4C8B-A4CE-52D7109D9156}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,19 +646,20 @@
     <col min="8" max="8" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="5" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" style="5" customWidth="1"/>
-    <col min="17" max="18" width="22.5703125" style="6" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" style="7" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" style="7" customWidth="1"/>
-    <col min="21" max="28" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.85546875" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="5" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" style="5" customWidth="1"/>
+    <col min="18" max="19" width="22.5703125" style="6" customWidth="1"/>
+    <col min="20" max="20" width="22.5703125" style="7" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" style="7" customWidth="1"/>
+    <col min="22" max="29" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -684,62 +690,65 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101.0625</v>
       </c>
@@ -770,43 +779,43 @@
       <c r="J2" t="s">
         <v>36</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="13">
         <v>0</v>
       </c>
-      <c r="L2" s="4">
-        <f t="shared" ref="L2:L11" ca="1" si="0">RANDBETWEEN(1000,10000)</f>
-        <v>9097</v>
-      </c>
-      <c r="M2" s="5">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <f t="shared" ref="M2:M11" ca="1" si="0">RANDBETWEEN(1000,10000)</f>
+        <v>8950</v>
+      </c>
+      <c r="N2" s="5">
         <f>(SUMIF(F2:F11,F2,F2:F11)/F2)/COUNT(F2:F11)</f>
         <v>0.2</v>
       </c>
-      <c r="N2" s="9">
+      <c r="O2" s="9">
         <v>29640</v>
       </c>
-      <c r="O2" s="10">
-        <f>M3</f>
+      <c r="P2" s="10">
+        <f>N3</f>
         <v>0.3</v>
       </c>
-      <c r="P2" s="11">
+      <c r="Q2" s="11">
         <f>6.62607*10^-34</f>
         <v>6.6260700000000011E-34</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="R2" s="6">
         <v>31179</v>
       </c>
-      <c r="R2" s="6">
+      <c r="S2" s="6">
         <v>31920</v>
       </c>
-      <c r="S2" s="7">
+      <c r="T2" s="7">
         <v>43950</v>
       </c>
-      <c r="T2" s="12">
+      <c r="U2" s="12">
         <v>43950</v>
       </c>
-      <c r="U2" t="s">
-        <v>37</v>
-      </c>
       <c r="V2" t="s">
         <v>37</v>
       </c>
@@ -828,8 +837,11 @@
       <c r="AB2" t="s">
         <v>37</v>
       </c>
+      <c r="AC2" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43102.449583333335</v>
       </c>
@@ -860,42 +872,42 @@
       <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="13">
         <v>123</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
+        <v>123</v>
+      </c>
+      <c r="M3" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>2571</v>
-      </c>
-      <c r="M3" s="5">
+        <v>2070</v>
+      </c>
+      <c r="N3" s="5">
         <f>(SUMIF(F2:F11,F3,F2:F11)/F3)/COUNT(F2:F11)</f>
         <v>0.3</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <v>29641</v>
       </c>
-      <c r="O3" s="10">
-        <f t="shared" ref="O3:O11" si="1">M3</f>
+      <c r="P3" s="10">
+        <f t="shared" ref="P3:P11" si="1">N3</f>
         <v>0.3</v>
       </c>
-      <c r="P3" s="11">
+      <c r="Q3" s="11">
         <f>3*10^-8</f>
         <v>3.0000000000000004E-8</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="R3" s="6">
         <v>31180</v>
       </c>
-      <c r="R3" s="6">
+      <c r="S3" s="6">
         <v>31921</v>
       </c>
-      <c r="S3" s="7">
+      <c r="T3" s="7">
         <v>43951</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>43951</v>
-      </c>
-      <c r="U3" t="s">
-        <v>41</v>
       </c>
       <c r="V3" t="s">
         <v>41</v>
@@ -918,8 +930,11 @@
       <c r="AB3" t="s">
         <v>41</v>
       </c>
+      <c r="AC3" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>SUM(A2,365)</f>
         <v>43466.0625</v>
@@ -956,43 +971,44 @@
       <c r="J4" t="s">
         <v>43</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="13">
         <f>SUM(15,0.5)</f>
         <v>15.5</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
+        <f>SUM(15,0.5)</f>
+        <v>15.5</v>
+      </c>
+      <c r="M4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>7149</v>
-      </c>
-      <c r="M4" s="5">
+        <v>6018</v>
+      </c>
+      <c r="N4" s="5">
         <f>(SUMIF(F2:F11,F4,F2:F11)/F4)/COUNT(F2:F11)</f>
         <v>0.1</v>
       </c>
-      <c r="N4" s="9">
+      <c r="O4" s="9">
         <v>29642</v>
       </c>
-      <c r="O4" s="10">
+      <c r="P4" s="10">
         <v>0.2857142857142857</v>
       </c>
-      <c r="P4" s="11">
+      <c r="Q4" s="11">
         <f>9.11*10^-31</f>
         <v>9.1100000000000003E-31</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="R4" s="6">
         <v>31181</v>
       </c>
-      <c r="R4" s="6">
+      <c r="S4" s="6">
         <v>31922</v>
       </c>
-      <c r="S4" s="7">
+      <c r="T4" s="7">
         <v>43952</v>
       </c>
-      <c r="T4" s="12">
+      <c r="U4" s="12">
         <v>43952</v>
       </c>
-      <c r="U4" t="s">
-        <v>37</v>
-      </c>
       <c r="V4" t="s">
         <v>37</v>
       </c>
@@ -1014,15 +1030,18 @@
       <c r="AB4" t="s">
         <v>37</v>
       </c>
+      <c r="AC4" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43104</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
@@ -1046,47 +1065,47 @@
       <c r="J5" t="s">
         <v>46</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="13">
         <v>35</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
+        <v>35</v>
+      </c>
+      <c r="M5" s="4">
         <v>7278</v>
       </c>
-      <c r="M5" s="5">
+      <c r="N5" s="5">
         <f>0.1</f>
         <v>0.1</v>
       </c>
-      <c r="N5" s="9">
-        <f>SUM(N4,1)</f>
+      <c r="O5" s="9">
+        <f>SUM(O4,1)</f>
         <v>29643</v>
       </c>
-      <c r="O5" s="5">
-        <f>M5+1</f>
+      <c r="P5" s="5">
+        <f>N5+1</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="P5" s="11">
+      <c r="Q5" s="11">
         <v>1.6730000000000002E-27</v>
-      </c>
-      <c r="Q5" s="6">
-        <f>Q4+1</f>
-        <v>31182</v>
       </c>
       <c r="R5" s="6">
         <f>R4+1</f>
+        <v>31182</v>
+      </c>
+      <c r="S5" s="6">
+        <f>S4+1</f>
         <v>31923</v>
       </c>
-      <c r="S5" s="7">
+      <c r="T5" s="7">
         <v>43953</v>
       </c>
-      <c r="T5" s="12">
+      <c r="U5" s="12">
         <v>43953</v>
       </c>
-      <c r="U5" t="str">
-        <f>SUBSTITUTE(U4,"CategoryA","CategoryC")</f>
+      <c r="V5" t="str">
+        <f>SUBSTITUTE(V4,"CategoryA","CategoryC")</f>
         <v>CategoryC</v>
-      </c>
-      <c r="V5" t="s">
-        <v>41</v>
       </c>
       <c r="W5" t="s">
         <v>41</v>
@@ -1106,15 +1125,18 @@
       <c r="AB5" t="s">
         <v>41</v>
       </c>
+      <c r="AC5" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43105</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
@@ -1138,44 +1160,44 @@
       <c r="J6" t="s">
         <v>49</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="13">
         <v>523523</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
+        <v>523523</v>
+      </c>
+      <c r="M6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>2940</v>
-      </c>
-      <c r="M6" s="5">
+        <v>7186</v>
+      </c>
+      <c r="N6" s="5">
         <f>(SUMIF(F2:F11,F6,F2:F11)/F6)/COUNT(F2:F11)</f>
         <v>0.3</v>
       </c>
-      <c r="N6" s="9">
+      <c r="O6" s="9">
         <v>29644</v>
       </c>
-      <c r="O6" s="10">
+      <c r="P6" s="10">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="P6" s="11">
+      <c r="Q6" s="11">
         <f>1.675*10^-27</f>
         <v>1.6750000000000003E-27</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="6">
         <v>31183</v>
       </c>
-      <c r="R6" s="6">
+      <c r="S6" s="6">
         <v>31924</v>
       </c>
-      <c r="S6" s="7">
-        <f>S4+1</f>
+      <c r="T6" s="7">
+        <f>T4+1</f>
         <v>43953</v>
       </c>
-      <c r="T6" s="12">
+      <c r="U6" s="12">
         <v>43954</v>
       </c>
-      <c r="U6" t="s">
-        <v>37</v>
-      </c>
       <c r="V6" t="s">
         <v>37</v>
       </c>
@@ -1197,8 +1219,11 @@
       <c r="AB6" t="s">
         <v>37</v>
       </c>
+      <c r="AC6" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43106</v>
       </c>
@@ -1229,43 +1254,43 @@
       <c r="J7" t="s">
         <v>52</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="13">
         <v>400</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
+        <v>400</v>
+      </c>
+      <c r="M7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6964</v>
-      </c>
-      <c r="M7" s="5">
+        <v>9924</v>
+      </c>
+      <c r="N7" s="5">
         <f>(SUMIF(F2:F11,F7,F2:F11)/F7)/COUNT(F2:F11)</f>
         <v>0.1</v>
       </c>
-      <c r="N7" s="9">
+      <c r="O7" s="9">
         <v>29645</v>
       </c>
-      <c r="O7" s="10">
+      <c r="P7" s="10">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="P7" s="11">
+      <c r="Q7" s="11">
         <f>1.673*10^-27</f>
         <v>1.6730000000000002E-27</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>31184</v>
       </c>
-      <c r="R7" s="6">
+      <c r="S7" s="6">
         <v>31925</v>
       </c>
-      <c r="S7" s="7">
+      <c r="T7" s="7">
         <v>43955</v>
       </c>
-      <c r="T7" s="12">
+      <c r="U7" s="12">
         <v>43955</v>
       </c>
-      <c r="U7" t="s">
-        <v>37</v>
-      </c>
       <c r="V7" t="s">
         <v>37</v>
       </c>
@@ -1287,8 +1312,11 @@
       <c r="AB7" t="s">
         <v>37</v>
       </c>
+      <c r="AC7" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43107</v>
       </c>
@@ -1319,42 +1347,42 @@
       <c r="J8" t="s">
         <v>55</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="13">
         <v>203</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
+        <v>203</v>
+      </c>
+      <c r="M8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>8133</v>
-      </c>
-      <c r="M8" s="5">
+        <v>6882</v>
+      </c>
+      <c r="N8" s="5">
         <f>(SUMIF(F2:F11,F8,F2:F11)/F8)/COUNT(F2:F11)</f>
         <v>0.1</v>
       </c>
-      <c r="N8" s="9">
+      <c r="O8" s="9">
         <v>29646</v>
       </c>
-      <c r="O8" s="10">
+      <c r="P8" s="10">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="P8" s="11">
+      <c r="Q8" s="11">
         <f>1.673*10^-27</f>
         <v>1.6730000000000002E-27</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>31185</v>
       </c>
-      <c r="R8" s="6">
+      <c r="S8" s="6">
         <v>31926</v>
       </c>
-      <c r="S8" s="7">
+      <c r="T8" s="7">
         <v>43956</v>
       </c>
-      <c r="T8" s="12">
+      <c r="U8" s="12">
         <v>43956</v>
-      </c>
-      <c r="U8" t="s">
-        <v>56</v>
       </c>
       <c r="V8" t="s">
         <v>56</v>
@@ -1377,8 +1405,11 @@
       <c r="AB8" t="s">
         <v>56</v>
       </c>
+      <c r="AC8" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43108</v>
       </c>
@@ -1409,43 +1440,43 @@
       <c r="J9" t="s">
         <v>59</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="13">
         <v>20</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
+        <v>20</v>
+      </c>
+      <c r="M9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6552</v>
-      </c>
-      <c r="M9" s="5">
+        <v>8403</v>
+      </c>
+      <c r="N9" s="5">
         <f>(SUMIF(F2:F11,F9,F2:F11)/F9)/COUNT(F2:F11)</f>
         <v>0.2</v>
       </c>
-      <c r="N9" s="9">
+      <c r="O9" s="9">
         <v>29647</v>
       </c>
-      <c r="O9" s="10">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="P9" s="11">
+      <c r="Q9" s="11">
         <f>1.673*10^-27</f>
         <v>1.6730000000000002E-27</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="6">
         <v>31186</v>
       </c>
-      <c r="R9" s="6">
+      <c r="S9" s="6">
         <v>31927</v>
       </c>
-      <c r="S9" s="7">
+      <c r="T9" s="7">
         <v>43957</v>
       </c>
-      <c r="T9" s="12">
+      <c r="U9" s="12">
         <v>43957</v>
       </c>
-      <c r="U9" t="s">
-        <v>37</v>
-      </c>
       <c r="V9" t="s">
         <v>37</v>
       </c>
@@ -1467,8 +1498,11 @@
       <c r="AB9" t="s">
         <v>37</v>
       </c>
+      <c r="AC9" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43109</v>
       </c>
@@ -1499,43 +1533,43 @@
       <c r="J10" t="s">
         <v>62</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="13">
         <v>3</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>8188</v>
-      </c>
-      <c r="M10" s="5">
+        <v>5305</v>
+      </c>
+      <c r="N10" s="5">
         <f>(SUMIF(F2:F11,F10,F2:F11)/F10)/COUNT(F2:F11)</f>
         <v>0.3</v>
       </c>
-      <c r="N10" s="9">
+      <c r="O10" s="9">
         <v>29648</v>
       </c>
-      <c r="O10" s="10">
+      <c r="P10" s="10">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="P10" s="11">
+      <c r="Q10" s="11">
         <f>1.673*10^-27</f>
         <v>1.6730000000000002E-27</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="6">
         <v>31187</v>
       </c>
-      <c r="R10" s="6">
+      <c r="S10" s="6">
         <v>31928</v>
       </c>
-      <c r="S10" s="7">
+      <c r="T10" s="7">
         <v>43958</v>
       </c>
-      <c r="T10" s="12">
+      <c r="U10" s="12">
         <v>43958</v>
       </c>
-      <c r="U10" t="s">
-        <v>37</v>
-      </c>
       <c r="V10" t="s">
         <v>37</v>
       </c>
@@ -1557,8 +1591,11 @@
       <c r="AB10" t="s">
         <v>37</v>
       </c>
+      <c r="AC10" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43110</v>
       </c>
@@ -1589,42 +1626,42 @@
       <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="13">
         <v>1</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>2256</v>
-      </c>
-      <c r="M11" s="5">
+        <v>5880</v>
+      </c>
+      <c r="N11" s="5">
         <f>(SUMIF(F2:F11,F11,F2:F11)/F11)/COUNT(F2:F11)</f>
         <v>0.1</v>
       </c>
-      <c r="N11" s="9">
+      <c r="O11" s="9">
         <v>29649</v>
       </c>
-      <c r="O11" s="10">
+      <c r="P11" s="10">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="P11" s="11">
+      <c r="Q11" s="11">
         <f>1.673*10^-27</f>
         <v>1.6730000000000002E-27</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="R11" s="6">
         <v>31188</v>
       </c>
-      <c r="R11" s="6">
+      <c r="S11" s="6">
         <v>31929</v>
       </c>
-      <c r="S11" s="7">
+      <c r="T11" s="7">
         <v>43959</v>
       </c>
-      <c r="T11" s="12">
+      <c r="U11" s="12">
         <v>43959</v>
-      </c>
-      <c r="U11" t="s">
-        <v>56</v>
       </c>
       <c r="V11" t="s">
         <v>56</v>
@@ -1645,6 +1682,9 @@
         <v>56</v>
       </c>
       <c r="AB11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC11" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1971,15 +2011,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E4532DD-54FD-4DB2-BD04-1DFA2187B2EF}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="3349f526-a3e5-45fb-8ad6-0535a314a9a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="45586092-62d1-4827-bb05-1abb442adc62"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>